<commit_message>
Fixed typo of duplicates in all-authors
</commit_message>
<xml_diff>
--- a/data/all-authors-3.0.xlsx
+++ b/data/all-authors-3.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="827">
   <si>
     <t>Paper ID</t>
   </si>
@@ -2477,16 +2477,7 @@
     <t>US0035</t>
   </si>
   <si>
-    <t xml:space="preserve">Susanne Bülow </t>
-  </si>
-  <si>
     <t>/l/ChengfeiLiu</t>
-  </si>
-  <si>
-    <t>Feng Gao</t>
-  </si>
-  <si>
-    <t>Irelad</t>
   </si>
   <si>
     <t>Maximilian Völker</t>
@@ -2758,8 +2749,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D609" totalsRowShown="0">
-  <autoFilter ref="A1:D609"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D602" totalsRowShown="0">
+  <autoFilter ref="A1:D602"/>
   <sortState ref="A2:D569">
     <sortCondition ref="A1:A569"/>
   </sortState>
@@ -3036,18 +3027,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D609"/>
+  <dimension ref="A1:D602"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A590" workbookViewId="0">
-      <selection activeCell="B508" sqref="B508"/>
+    <sheetView tabSelected="1" topLeftCell="A524" workbookViewId="0">
+      <selection activeCell="A539" sqref="A539:XFD542"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -10542,125 +10533,125 @@
     </row>
     <row r="536" spans="1:4">
       <c r="A536" s="15">
-        <v>2352968</v>
+        <v>2353028</v>
       </c>
       <c r="B536" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C536" s="16" t="s">
-        <v>50</v>
+        <v>105</v>
+      </c>
+      <c r="C536" s="3" t="s">
+        <v>807</v>
       </c>
       <c r="D536" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="537" spans="1:4">
       <c r="A537" s="15">
-        <v>2352968</v>
-      </c>
-      <c r="B537" s="3" t="s">
-        <v>38</v>
+        <v>2353028</v>
+      </c>
+      <c r="B537" s="16" t="s">
+        <v>817</v>
       </c>
       <c r="C537" s="3" t="s">
-        <v>817</v>
+        <v>108</v>
       </c>
       <c r="D537" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="538" spans="1:4">
       <c r="A538" s="15">
-        <v>2352968</v>
+        <v>2353028</v>
       </c>
       <c r="B538" s="16" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="C538" s="16" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="D538" t="s">
-        <v>659</v>
+        <v>681</v>
       </c>
     </row>
     <row r="539" spans="1:4">
       <c r="A539" s="15">
-        <v>2353028</v>
+        <v>2353203</v>
       </c>
       <c r="B539" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C539" s="3" t="s">
-        <v>807</v>
+        <v>759</v>
+      </c>
+      <c r="C539" s="16" t="s">
+        <v>760</v>
       </c>
       <c r="D539" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="540" spans="1:4">
       <c r="A540" s="15">
-        <v>2353028</v>
+        <v>2353203</v>
       </c>
       <c r="B540" s="16" t="s">
+        <v>761</v>
+      </c>
+      <c r="C540" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="C540" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="D540" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="541" spans="1:4">
       <c r="A541" s="15">
-        <v>2353028</v>
+        <v>2353203</v>
       </c>
       <c r="B541" s="16" t="s">
-        <v>109</v>
+        <v>477</v>
       </c>
       <c r="C541" s="16" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D541" t="s">
-        <v>681</v>
+        <v>659</v>
       </c>
     </row>
     <row r="542" spans="1:4">
       <c r="A542" s="15">
-        <v>2353177</v>
-      </c>
-      <c r="B542" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C542" s="3" t="s">
-        <v>819</v>
+        <v>2353211</v>
+      </c>
+      <c r="B542" s="16" t="s">
+        <v>762</v>
+      </c>
+      <c r="C542" s="16" t="s">
+        <v>763</v>
       </c>
       <c r="D542" t="s">
-        <v>820</v>
+        <v>662</v>
       </c>
     </row>
     <row r="543" spans="1:4">
       <c r="A543" s="15">
-        <v>2353177</v>
-      </c>
-      <c r="B543" s="16" t="s">
-        <v>240</v>
+        <v>2353211</v>
+      </c>
+      <c r="B543" s="3" t="s">
+        <v>764</v>
       </c>
       <c r="C543" s="16" t="s">
-        <v>241</v>
+        <v>765</v>
       </c>
       <c r="D543" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="544" spans="1:4">
       <c r="A544" s="15">
-        <v>2353177</v>
-      </c>
-      <c r="B544" s="16" t="s">
-        <v>242</v>
+        <v>2353211</v>
+      </c>
+      <c r="B544" s="3" t="s">
+        <v>766</v>
       </c>
       <c r="C544" s="16" t="s">
-        <v>243</v>
+        <v>767</v>
       </c>
       <c r="D544" t="s">
         <v>705</v>
@@ -10668,83 +10659,83 @@
     </row>
     <row r="545" spans="1:4">
       <c r="A545" s="15">
-        <v>2353177</v>
+        <v>2353212</v>
       </c>
       <c r="B545" s="3" t="s">
-        <v>244</v>
+        <v>9</v>
       </c>
       <c r="C545" s="16" t="s">
-        <v>245</v>
+        <v>10</v>
       </c>
       <c r="D545" t="s">
-        <v>705</v>
+        <v>654</v>
       </c>
     </row>
     <row r="546" spans="1:4">
       <c r="A546" s="15">
-        <v>2353203</v>
-      </c>
-      <c r="B546" s="3" t="s">
-        <v>759</v>
+        <v>2353212</v>
+      </c>
+      <c r="B546" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="C546" s="16" t="s">
-        <v>760</v>
+        <v>12</v>
       </c>
       <c r="D546" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
     </row>
     <row r="547" spans="1:4">
       <c r="A547" s="15">
-        <v>2353203</v>
+        <v>2353212</v>
       </c>
       <c r="B547" s="16" t="s">
-        <v>761</v>
-      </c>
-      <c r="C547" s="3" t="s">
-        <v>821</v>
+        <v>13</v>
+      </c>
+      <c r="C547" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D547" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
     </row>
     <row r="548" spans="1:4">
       <c r="A548" s="15">
-        <v>2353203</v>
-      </c>
-      <c r="B548" s="16" t="s">
-        <v>477</v>
-      </c>
-      <c r="C548" s="16" t="s">
-        <v>88</v>
+        <v>2353249</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C548" s="3" t="s">
+        <v>820</v>
       </c>
       <c r="D548" t="s">
-        <v>659</v>
+        <v>705</v>
       </c>
     </row>
     <row r="549" spans="1:4">
       <c r="A549" s="15">
-        <v>2353211</v>
-      </c>
-      <c r="B549" s="16" t="s">
-        <v>762</v>
+        <v>2353249</v>
+      </c>
+      <c r="B549" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="C549" s="16" t="s">
-        <v>763</v>
+        <v>243</v>
       </c>
       <c r="D549" t="s">
-        <v>662</v>
+        <v>705</v>
       </c>
     </row>
     <row r="550" spans="1:4">
       <c r="A550" s="15">
-        <v>2353211</v>
-      </c>
-      <c r="B550" s="3" t="s">
-        <v>764</v>
+        <v>2353249</v>
+      </c>
+      <c r="B550" s="16" t="s">
+        <v>821</v>
       </c>
       <c r="C550" s="16" t="s">
-        <v>765</v>
+        <v>808</v>
       </c>
       <c r="D550" t="s">
         <v>822</v>
@@ -10752,111 +10743,111 @@
     </row>
     <row r="551" spans="1:4">
       <c r="A551" s="15">
-        <v>2353211</v>
+        <v>2614321</v>
       </c>
       <c r="B551" s="3" t="s">
-        <v>766</v>
-      </c>
-      <c r="C551" s="16" t="s">
-        <v>767</v>
+        <v>105</v>
+      </c>
+      <c r="C551" s="3" t="s">
+        <v>807</v>
       </c>
       <c r="D551" t="s">
-        <v>705</v>
+        <v>660</v>
       </c>
     </row>
     <row r="552" spans="1:4">
       <c r="A552" s="15">
-        <v>2353212</v>
+        <v>2614321</v>
       </c>
       <c r="B552" s="3" t="s">
-        <v>9</v>
+        <v>768</v>
       </c>
       <c r="C552" s="16" t="s">
-        <v>10</v>
+        <v>769</v>
       </c>
       <c r="D552" t="s">
-        <v>654</v>
+        <v>708</v>
       </c>
     </row>
     <row r="553" spans="1:4">
       <c r="A553" s="15">
-        <v>2353212</v>
-      </c>
-      <c r="B553" s="16" t="s">
-        <v>11</v>
+        <v>2614321</v>
+      </c>
+      <c r="B553" s="3" t="s">
+        <v>770</v>
       </c>
       <c r="C553" s="16" t="s">
-        <v>12</v>
+        <v>771</v>
       </c>
       <c r="D553" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="554" spans="1:4">
       <c r="A554" s="15">
-        <v>2353212</v>
+        <v>2614324</v>
       </c>
       <c r="B554" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C554" s="16" t="s">
-        <v>14</v>
+        <v>105</v>
+      </c>
+      <c r="C554" s="3" t="s">
+        <v>807</v>
       </c>
       <c r="D554" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
     </row>
     <row r="555" spans="1:4">
       <c r="A555" s="15">
-        <v>2353249</v>
-      </c>
-      <c r="B555" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C555" s="3" t="s">
-        <v>823</v>
+        <v>2614324</v>
+      </c>
+      <c r="B555" s="16" t="s">
+        <v>768</v>
+      </c>
+      <c r="C555" s="16" t="s">
+        <v>769</v>
       </c>
       <c r="D555" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="556" spans="1:4">
       <c r="A556" s="15">
-        <v>2353249</v>
-      </c>
-      <c r="B556" s="1" t="s">
-        <v>242</v>
+        <v>2614324</v>
+      </c>
+      <c r="B556" s="16" t="s">
+        <v>770</v>
       </c>
       <c r="C556" s="16" t="s">
-        <v>243</v>
+        <v>771</v>
       </c>
       <c r="D556" t="s">
-        <v>705</v>
+        <v>652</v>
       </c>
     </row>
     <row r="557" spans="1:4">
       <c r="A557" s="15">
-        <v>2353249</v>
+        <v>2614324</v>
       </c>
       <c r="B557" s="16" t="s">
+        <v>772</v>
+      </c>
+      <c r="C557" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="D557" t="s">
         <v>824</v>
-      </c>
-      <c r="C557" s="16" t="s">
-        <v>808</v>
-      </c>
-      <c r="D557" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="558" spans="1:4">
       <c r="A558" s="15">
-        <v>2614321</v>
-      </c>
-      <c r="B558" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C558" s="3" t="s">
-        <v>807</v>
+        <v>2614324</v>
+      </c>
+      <c r="B558" s="16" t="s">
+        <v>773</v>
+      </c>
+      <c r="C558" s="16" t="s">
+        <v>774</v>
       </c>
       <c r="D558" t="s">
         <v>660</v>
@@ -10864,147 +10855,147 @@
     </row>
     <row r="559" spans="1:4">
       <c r="A559" s="15">
-        <v>2614321</v>
-      </c>
-      <c r="B559" s="3" t="s">
-        <v>768</v>
+        <v>2614539</v>
+      </c>
+      <c r="B559" s="16" t="s">
+        <v>775</v>
       </c>
       <c r="C559" s="16" t="s">
-        <v>769</v>
+        <v>776</v>
       </c>
       <c r="D559" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="560" spans="1:4">
       <c r="A560" s="15">
-        <v>2614321</v>
-      </c>
-      <c r="B560" s="3" t="s">
-        <v>770</v>
+        <v>2614539</v>
+      </c>
+      <c r="B560" s="16" t="s">
+        <v>777</v>
       </c>
       <c r="C560" s="16" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
       <c r="D560" t="s">
-        <v>652</v>
+        <v>709</v>
       </c>
     </row>
     <row r="561" spans="1:4">
       <c r="A561" s="15">
-        <v>2614324</v>
+        <v>2614539</v>
       </c>
       <c r="B561" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C561" s="3" t="s">
-        <v>807</v>
+        <v>779</v>
+      </c>
+      <c r="C561" s="16" t="s">
+        <v>780</v>
       </c>
       <c r="D561" t="s">
-        <v>660</v>
+        <v>825</v>
       </c>
     </row>
     <row r="562" spans="1:4">
       <c r="A562" s="15">
-        <v>2614324</v>
+        <v>2614833</v>
       </c>
       <c r="B562" s="16" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="C562" s="16" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="D562" t="s">
-        <v>708</v>
+        <v>682</v>
       </c>
     </row>
     <row r="563" spans="1:4">
       <c r="A563" s="15">
-        <v>2614324</v>
+        <v>2614833</v>
       </c>
       <c r="B563" s="16" t="s">
-        <v>770</v>
+        <v>783</v>
       </c>
       <c r="C563" s="16" t="s">
-        <v>771</v>
+        <v>784</v>
       </c>
       <c r="D563" t="s">
-        <v>652</v>
+        <v>682</v>
       </c>
     </row>
     <row r="564" spans="1:4">
       <c r="A564" s="15">
-        <v>2614324</v>
+        <v>2614909</v>
       </c>
       <c r="B564" s="16" t="s">
-        <v>772</v>
-      </c>
-      <c r="C564" s="3" t="s">
-        <v>826</v>
+        <v>781</v>
+      </c>
+      <c r="C564" s="16" t="s">
+        <v>782</v>
       </c>
       <c r="D564" t="s">
-        <v>827</v>
+        <v>682</v>
       </c>
     </row>
     <row r="565" spans="1:4">
       <c r="A565" s="15">
-        <v>2614324</v>
+        <v>2614909</v>
       </c>
       <c r="B565" s="16" t="s">
-        <v>773</v>
+        <v>785</v>
       </c>
       <c r="C565" s="16" t="s">
-        <v>774</v>
+        <v>786</v>
       </c>
       <c r="D565" t="s">
-        <v>660</v>
+        <v>682</v>
       </c>
     </row>
     <row r="566" spans="1:4">
       <c r="A566" s="15">
-        <v>2614539</v>
+        <v>2614909</v>
       </c>
       <c r="B566" s="16" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="C566" s="16" t="s">
-        <v>776</v>
+        <v>788</v>
       </c>
       <c r="D566" t="s">
-        <v>709</v>
+        <v>682</v>
       </c>
     </row>
     <row r="567" spans="1:4">
       <c r="A567" s="15">
-        <v>2614539</v>
+        <v>2614909</v>
       </c>
       <c r="B567" s="16" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="C567" s="16" t="s">
-        <v>778</v>
+        <v>790</v>
       </c>
       <c r="D567" t="s">
-        <v>709</v>
+        <v>682</v>
       </c>
     </row>
     <row r="568" spans="1:4">
       <c r="A568" s="15">
-        <v>2614539</v>
+        <v>2614909</v>
       </c>
       <c r="B568" s="16" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="C568" s="16" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="D568" t="s">
-        <v>828</v>
+        <v>682</v>
       </c>
     </row>
     <row r="569" spans="1:4">
       <c r="A569" s="15">
-        <v>2614833</v>
+        <v>2644180</v>
       </c>
       <c r="B569" s="16" t="s">
         <v>781</v>
@@ -11018,13 +11009,13 @@
     </row>
     <row r="570" spans="1:4">
       <c r="A570" s="15">
-        <v>2614833</v>
+        <v>2644180</v>
       </c>
       <c r="B570" s="16" t="s">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c r="C570" s="16" t="s">
-        <v>784</v>
+        <v>790</v>
       </c>
       <c r="D570" t="s">
         <v>682</v>
@@ -11032,13 +11023,13 @@
     </row>
     <row r="571" spans="1:4">
       <c r="A571" s="15">
-        <v>2614909</v>
+        <v>2644180</v>
       </c>
       <c r="B571" s="16" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="C571" s="16" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="D571" t="s">
         <v>682</v>
@@ -11046,13 +11037,13 @@
     </row>
     <row r="572" spans="1:4">
       <c r="A572" s="15">
-        <v>2614909</v>
+        <v>2644180</v>
       </c>
       <c r="B572" s="16" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C572" s="16" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="D572" t="s">
         <v>682</v>
@@ -11060,13 +11051,13 @@
     </row>
     <row r="573" spans="1:4">
       <c r="A573" s="15">
-        <v>2614909</v>
+        <v>2644180</v>
       </c>
       <c r="B573" s="16" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C573" s="16" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="D573" t="s">
         <v>682</v>
@@ -11074,13 +11065,13 @@
     </row>
     <row r="574" spans="1:4">
       <c r="A574" s="15">
-        <v>2614909</v>
+        <v>2644180</v>
       </c>
       <c r="B574" s="16" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C574" s="16" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="D574" t="s">
         <v>682</v>
@@ -11088,111 +11079,111 @@
     </row>
     <row r="575" spans="1:4">
       <c r="A575" s="15">
-        <v>2614909</v>
-      </c>
-      <c r="B575" s="16" t="s">
-        <v>783</v>
+        <v>2644233</v>
+      </c>
+      <c r="B575" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="C575" s="16" t="s">
-        <v>784</v>
+        <v>56</v>
       </c>
       <c r="D575" t="s">
-        <v>682</v>
+        <v>659</v>
       </c>
     </row>
     <row r="576" spans="1:4">
       <c r="A576" s="15">
-        <v>2644180</v>
-      </c>
-      <c r="B576" s="16" t="s">
-        <v>781</v>
+        <v>2644233</v>
+      </c>
+      <c r="B576" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C576" s="16" t="s">
-        <v>782</v>
+        <v>126</v>
       </c>
       <c r="D576" t="s">
-        <v>682</v>
+        <v>653</v>
       </c>
     </row>
     <row r="577" spans="1:4">
       <c r="A577" s="15">
-        <v>2644180</v>
+        <v>2644233</v>
       </c>
       <c r="B577" s="16" t="s">
-        <v>789</v>
+        <v>292</v>
       </c>
       <c r="C577" s="16" t="s">
-        <v>790</v>
+        <v>293</v>
       </c>
       <c r="D577" t="s">
-        <v>682</v>
+        <v>727</v>
       </c>
     </row>
     <row r="578" spans="1:4">
       <c r="A578" s="15">
-        <v>2644180</v>
+        <v>2644233</v>
       </c>
       <c r="B578" s="16" t="s">
-        <v>785</v>
+        <v>477</v>
       </c>
       <c r="C578" s="16" t="s">
-        <v>786</v>
+        <v>88</v>
       </c>
       <c r="D578" t="s">
-        <v>682</v>
+        <v>659</v>
       </c>
     </row>
     <row r="579" spans="1:4">
       <c r="A579" s="15">
-        <v>2644180</v>
+        <v>2644233</v>
       </c>
       <c r="B579" s="16" t="s">
-        <v>787</v>
+        <v>57</v>
       </c>
       <c r="C579" s="16" t="s">
-        <v>788</v>
+        <v>58</v>
       </c>
       <c r="D579" t="s">
-        <v>682</v>
+        <v>659</v>
       </c>
     </row>
     <row r="580" spans="1:4">
       <c r="A580" s="15">
-        <v>2644180</v>
+        <v>2644233</v>
       </c>
       <c r="B580" s="16" t="s">
-        <v>783</v>
-      </c>
-      <c r="C580" s="16" t="s">
-        <v>784</v>
+        <v>45</v>
+      </c>
+      <c r="C580" s="3" t="s">
+        <v>826</v>
       </c>
       <c r="D580" t="s">
-        <v>682</v>
+        <v>659</v>
       </c>
     </row>
     <row r="581" spans="1:4">
       <c r="A581" s="15">
-        <v>2644180</v>
+        <v>2644233</v>
       </c>
       <c r="B581" s="16" t="s">
-        <v>791</v>
+        <v>294</v>
       </c>
       <c r="C581" s="16" t="s">
-        <v>792</v>
+        <v>295</v>
       </c>
       <c r="D581" t="s">
-        <v>682</v>
+        <v>727</v>
       </c>
     </row>
     <row r="582" spans="1:4">
       <c r="A582" s="15">
         <v>2644233</v>
       </c>
-      <c r="B582" s="3" t="s">
-        <v>55</v>
+      <c r="B582" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="C582" s="16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D582" t="s">
         <v>659</v>
@@ -11202,165 +11193,165 @@
       <c r="A583" s="15">
         <v>2644233</v>
       </c>
-      <c r="B583" s="3" t="s">
-        <v>125</v>
+      <c r="B583" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="C583" s="16" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="D583" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
     </row>
     <row r="584" spans="1:4">
       <c r="A584" s="15">
-        <v>2644233</v>
-      </c>
-      <c r="B584" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="C584" s="16" t="s">
-        <v>293</v>
+        <v>2644405</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C584" s="3" t="s">
+        <v>820</v>
       </c>
       <c r="D584" t="s">
-        <v>727</v>
+        <v>705</v>
       </c>
     </row>
     <row r="585" spans="1:4">
       <c r="A585" s="15">
-        <v>2644233</v>
-      </c>
-      <c r="B585" s="16" t="s">
-        <v>477</v>
+        <v>2644405</v>
+      </c>
+      <c r="B585" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="C585" s="16" t="s">
-        <v>88</v>
+        <v>243</v>
       </c>
       <c r="D585" t="s">
-        <v>659</v>
+        <v>705</v>
       </c>
     </row>
     <row r="586" spans="1:4">
       <c r="A586" s="15">
-        <v>2644233</v>
+        <v>2644431</v>
       </c>
       <c r="B586" s="16" t="s">
-        <v>57</v>
+        <v>204</v>
       </c>
       <c r="C586" s="16" t="s">
-        <v>58</v>
+        <v>205</v>
       </c>
       <c r="D586" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="587" spans="1:4">
       <c r="A587" s="15">
-        <v>2644233</v>
+        <v>2644431</v>
       </c>
       <c r="B587" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C587" s="3" t="s">
-        <v>829</v>
+        <v>125</v>
+      </c>
+      <c r="C587" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="D587" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="588" spans="1:4">
       <c r="A588" s="15">
-        <v>2644233</v>
+        <v>2644431</v>
       </c>
       <c r="B588" s="16" t="s">
-        <v>294</v>
+        <v>57</v>
       </c>
       <c r="C588" s="16" t="s">
-        <v>295</v>
+        <v>58</v>
       </c>
       <c r="D588" t="s">
-        <v>727</v>
+        <v>659</v>
       </c>
     </row>
     <row r="589" spans="1:4">
       <c r="A589" s="15">
-        <v>2644233</v>
+        <v>2644431</v>
       </c>
       <c r="B589" s="16" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="C589" s="16" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="D589" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="590" spans="1:4">
       <c r="A590" s="15">
-        <v>2644233</v>
+        <v>2644431</v>
       </c>
       <c r="B590" s="16" t="s">
-        <v>49</v>
+        <v>208</v>
       </c>
       <c r="C590" s="16" t="s">
-        <v>50</v>
+        <v>209</v>
       </c>
       <c r="D590" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="591" spans="1:4">
       <c r="A591" s="15">
-        <v>2644405</v>
-      </c>
-      <c r="B591" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C591" s="3" t="s">
-        <v>823</v>
+        <v>2644581</v>
+      </c>
+      <c r="B591" s="16" t="s">
+        <v>793</v>
+      </c>
+      <c r="C591" s="16" t="s">
+        <v>794</v>
       </c>
       <c r="D591" t="s">
-        <v>705</v>
+        <v>653</v>
       </c>
     </row>
     <row r="592" spans="1:4">
       <c r="A592" s="15">
-        <v>2644405</v>
-      </c>
-      <c r="B592" s="1" t="s">
-        <v>242</v>
+        <v>2644581</v>
+      </c>
+      <c r="B592" s="16" t="s">
+        <v>212</v>
       </c>
       <c r="C592" s="16" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D592" t="s">
-        <v>705</v>
+        <v>724</v>
       </c>
     </row>
     <row r="593" spans="1:4">
       <c r="A593" s="15">
-        <v>2644431</v>
+        <v>2644581</v>
       </c>
       <c r="B593" s="16" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="C593" s="16" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="D593" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="594" spans="1:4">
       <c r="A594" s="15">
-        <v>2644431</v>
+        <v>2644581</v>
       </c>
       <c r="B594" s="16" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
       <c r="C594" s="16" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
       <c r="D594" t="s">
         <v>653</v>
@@ -11368,211 +11359,113 @@
     </row>
     <row r="595" spans="1:4">
       <c r="A595" s="15">
-        <v>2644431</v>
+        <v>2644581</v>
       </c>
       <c r="B595" s="16" t="s">
-        <v>57</v>
+        <v>220</v>
       </c>
       <c r="C595" s="16" t="s">
-        <v>58</v>
+        <v>221</v>
       </c>
       <c r="D595" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="596" spans="1:4">
       <c r="A596" s="15">
-        <v>2644431</v>
+        <v>3343996</v>
       </c>
       <c r="B596" s="16" t="s">
-        <v>127</v>
+        <v>795</v>
       </c>
       <c r="C596" s="16" t="s">
-        <v>128</v>
+        <v>796</v>
       </c>
       <c r="D596" t="s">
-        <v>655</v>
+        <v>705</v>
       </c>
     </row>
     <row r="597" spans="1:4">
       <c r="A597" s="15">
-        <v>2644431</v>
+        <v>3343996</v>
       </c>
       <c r="B597" s="16" t="s">
-        <v>208</v>
+        <v>766</v>
       </c>
       <c r="C597" s="16" t="s">
-        <v>209</v>
+        <v>767</v>
       </c>
       <c r="D597" t="s">
-        <v>655</v>
+        <v>705</v>
       </c>
     </row>
     <row r="598" spans="1:4">
       <c r="A598" s="15">
-        <v>2644581</v>
+        <v>3343998</v>
       </c>
       <c r="B598" s="16" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="C598" s="16" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="D598" t="s">
-        <v>653</v>
+        <v>705</v>
       </c>
     </row>
     <row r="599" spans="1:4">
       <c r="A599" s="15">
-        <v>2644581</v>
+        <v>3343998</v>
       </c>
       <c r="B599" s="16" t="s">
-        <v>212</v>
+        <v>797</v>
       </c>
       <c r="C599" s="16" t="s">
-        <v>213</v>
+        <v>798</v>
       </c>
       <c r="D599" t="s">
-        <v>724</v>
+        <v>705</v>
       </c>
     </row>
     <row r="600" spans="1:4">
       <c r="A600" s="15">
-        <v>2644581</v>
+        <v>3343998</v>
       </c>
       <c r="B600" s="16" t="s">
-        <v>216</v>
+        <v>766</v>
       </c>
       <c r="C600" s="16" t="s">
-        <v>217</v>
+        <v>767</v>
       </c>
       <c r="D600" t="s">
-        <v>653</v>
+        <v>705</v>
       </c>
     </row>
     <row r="601" spans="1:4">
       <c r="A601" s="15">
-        <v>2644581</v>
+        <v>3343998</v>
       </c>
       <c r="B601" s="16" t="s">
-        <v>222</v>
+        <v>799</v>
       </c>
       <c r="C601" s="16" t="s">
-        <v>223</v>
+        <v>800</v>
       </c>
       <c r="D601" t="s">
-        <v>653</v>
+        <v>705</v>
       </c>
     </row>
     <row r="602" spans="1:4">
-      <c r="A602" s="15">
-        <v>2644581</v>
-      </c>
-      <c r="B602" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="C602" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="D602" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="603" spans="1:4">
-      <c r="A603" s="15">
-        <v>3343996</v>
-      </c>
-      <c r="B603" s="16" t="s">
-        <v>795</v>
-      </c>
-      <c r="C603" s="16" t="s">
-        <v>796</v>
-      </c>
-      <c r="D603" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="604" spans="1:4">
-      <c r="A604" s="15">
-        <v>3343996</v>
-      </c>
-      <c r="B604" s="16" t="s">
-        <v>766</v>
-      </c>
-      <c r="C604" s="16" t="s">
-        <v>767</v>
-      </c>
-      <c r="D604" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="605" spans="1:4">
-      <c r="A605" s="15">
+      <c r="A602" s="17">
         <v>3343998</v>
       </c>
-      <c r="B605" s="16" t="s">
-        <v>795</v>
-      </c>
-      <c r="C605" s="16" t="s">
-        <v>796</v>
-      </c>
-      <c r="D605" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="606" spans="1:4">
-      <c r="A606" s="15">
-        <v>3343998</v>
-      </c>
-      <c r="B606" s="16" t="s">
-        <v>797</v>
-      </c>
-      <c r="C606" s="16" t="s">
-        <v>798</v>
-      </c>
-      <c r="D606" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="607" spans="1:4">
-      <c r="A607" s="15">
-        <v>3343998</v>
-      </c>
-      <c r="B607" s="16" t="s">
-        <v>766</v>
-      </c>
-      <c r="C607" s="16" t="s">
-        <v>767</v>
-      </c>
-      <c r="D607" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="608" spans="1:4">
-      <c r="A608" s="15">
-        <v>3343998</v>
-      </c>
-      <c r="B608" s="16" t="s">
-        <v>799</v>
-      </c>
-      <c r="C608" s="16" t="s">
-        <v>800</v>
-      </c>
-      <c r="D608" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="609" spans="1:4">
-      <c r="A609" s="17">
-        <v>3343998</v>
-      </c>
-      <c r="B609" s="18" t="s">
+      <c r="B602" s="18" t="s">
         <v>801</v>
       </c>
-      <c r="C609" s="18" t="s">
+      <c r="C602" s="18" t="s">
         <v>802</v>
       </c>
-      <c r="D609" s="12" t="s">
+      <c r="D602" s="12" t="s">
         <v>705</v>
       </c>
     </row>

</xml_diff>